<commit_message>
Fix : Tool ARP
</commit_message>
<xml_diff>
--- a/public/TEMPLATE_ARP - Copy.xlsx
+++ b/public/TEMPLATE_ARP - Copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000" tabRatio="742" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,8 @@
     <sheet name="TC" sheetId="6" r:id="rId6"/>
     <sheet name="DOM" sheetId="7" r:id="rId7"/>
     <sheet name="NGRS" sheetId="8" r:id="rId8"/>
-    <sheet name="FORMAT_UPDATE_GUI" sheetId="9" r:id="rId9"/>
+    <sheet name="FORMAT_UPDATE_GUI_ARP" sheetId="9" r:id="rId9"/>
+    <sheet name="FORMAT_UPDATE_GUI_AP_BYU_AP" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1187,7 +1188,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1217,13 +1220,41 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;L
+&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12037037037037" defaultRowHeight="14.4"/>
@@ -1315,7 +1346,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1377,7 +1410,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1414,7 +1449,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:J359"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1691,7 +1728,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:E254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2745,7 +2784,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2805,7 +2846,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2858,11 +2901,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4"/>

</xml_diff>